<commit_message>
Backup, Se crearon los Edit Add new Truth Items
</commit_message>
<xml_diff>
--- a/src/main/resources/xls/SuiteTruthItemsAndroid.xlsx
+++ b/src/main/resources/xls/SuiteTruthItemsAndroid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0" showInkAnnotation="0"/>
   <bookViews>
-    <workbookView firstSheet="7" tabRatio="500" windowHeight="15940" windowWidth="35680" xWindow="-36500" yWindow="4340"/>
+    <workbookView tabRatio="500" windowHeight="15940" windowWidth="35680" xWindow="-37060" yWindow="4260"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" r:id="rId1" sheetId="1"/>
@@ -18,6 +18,10 @@
     <sheet name="TestChangePrimaryIndAndroid" r:id="rId9" sheetId="11"/>
     <sheet name="TestChangePrimaryTechAndroid" r:id="rId10" sheetId="12"/>
     <sheet name="TestChangePrimaryProdAndroid" r:id="rId11" sheetId="13"/>
+    <sheet name="TestAddMoreIndustryAndroid" r:id="rId12" sheetId="14"/>
+    <sheet name="TestAddMoreRoleAndroid" r:id="rId13" sheetId="15"/>
+    <sheet name="TestAddMoreTechAndroid" r:id="rId14" sheetId="16"/>
+    <sheet name="TestAddMoreProductAndroid" r:id="rId15" sheetId="17"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -73,9 +77,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>selectProjectAndroidTSD</t>
-  </si>
-  <si>
     <t>App was able to login</t>
   </si>
   <si>
@@ -145,16 +146,58 @@
     <t>Validate thet the Primary can change for Product</t>
   </si>
   <si>
+    <t>Primary Role was found and changed</t>
+  </si>
+  <si>
+    <t>Primary industry was found and changed</t>
+  </si>
+  <si>
+    <t>Primary Technology was found and changed</t>
+  </si>
+  <si>
+    <t>Primary Prodcut was found and changed</t>
+  </si>
+  <si>
+    <t>TestAddMoreIndustryAndroid</t>
+  </si>
+  <si>
+    <t>TestAddMoreRoleAndroid</t>
+  </si>
+  <si>
+    <t>TestAddMoreTechAndroid</t>
+  </si>
+  <si>
+    <t>TestAddMoreProductAndroid</t>
+  </si>
+  <si>
+    <t>Test to add more Industry</t>
+  </si>
+  <si>
+    <t>Test to add more Roles</t>
+  </si>
+  <si>
+    <t>Test to add more Technology</t>
+  </si>
+  <si>
+    <t>Test to add more Product</t>
+  </si>
+  <si>
     <t>FAIL</t>
   </si>
   <si>
-    <t>Primary Role wasn't found and changed</t>
-  </si>
-  <si>
-    <t>Primary Role was found and changed</t>
-  </si>
-  <si>
-    <t>Primary industry was found and changed</t>
+    <t>ADO.NET tag wasn't found</t>
+  </si>
+  <si>
+    <t>Architects - Technical tag was found</t>
+  </si>
+  <si>
+    <t>Social &amp; Enterprise Mobility tag wasn't found</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence / Robotics tag wasn't found</t>
+  </si>
+  <si>
+    <t>Social &amp; Enterprise Mobility tag was found</t>
   </si>
 </sst>
 </file>
@@ -235,9 +278,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
@@ -268,7 +315,7 @@
     <xf applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="26">
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="3"/>
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="4"/>
@@ -289,6 +336,10 @@
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="19"/>
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="20"/>
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="21"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="22"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="23"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="24"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="25"/>
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
@@ -619,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -662,10 +713,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -676,10 +727,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -690,10 +741,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -704,10 +755,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -718,10 +769,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -729,10 +780,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -743,10 +794,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -757,24 +808,86 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -801,7 +914,8 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -838,13 +952,17 @@
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -872,7 +990,8 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="35.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -909,13 +1028,322 @@
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+  </hyperlinks>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.1640625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>18</v>
       </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+  </hyperlinks>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.76953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.23828125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+  </hyperlinks>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.76953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="37.57421875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+  </hyperlinks>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.76953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.23828125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -932,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -981,17 +1409,20 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1058,16 +1489,16 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1135,16 +1566,16 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1212,7 +1643,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -1221,7 +1652,7 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1242,7 +1673,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1288,7 +1719,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
@@ -1297,7 +1728,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1305,6 +1736,7 @@
     <hyperlink r:id="rId1" ref="B2"/>
   </hyperlinks>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1362,7 +1794,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
@@ -1397,8 +1829,8 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.76953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="33.24609375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="31.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1435,7 +1867,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
@@ -1444,7 +1876,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1473,8 +1905,8 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.76953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.23828125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="34.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1511,7 +1943,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
@@ -1520,7 +1952,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created Add new Tags for IOS
</commit_message>
<xml_diff>
--- a/src/main/resources/xls/SuiteTruthItemsAndroid.xlsx
+++ b/src/main/resources/xls/SuiteTruthItemsAndroid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0" showInkAnnotation="0"/>
   <bookViews>
-    <workbookView tabRatio="500" windowHeight="15940" windowWidth="35680" xWindow="-37060" yWindow="4260"/>
+    <workbookView tabRatio="500" windowHeight="15940" windowWidth="35680" xWindow="-48820" yWindow="1640"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" r:id="rId1" sheetId="1"/>
@@ -22,6 +22,13 @@
     <sheet name="TestAddMoreRoleAndroid" r:id="rId13" sheetId="15"/>
     <sheet name="TestAddMoreTechAndroid" r:id="rId14" sheetId="16"/>
     <sheet name="TestAddMoreProductAndroid" r:id="rId15" sheetId="17"/>
+    <sheet name="NewAnswerQ1Android" r:id="rId16" sheetId="24"/>
+    <sheet name="NewAnswerQ2Android" r:id="rId17" sheetId="22"/>
+    <sheet name="NewAnswerQ3Android" r:id="rId18" sheetId="23"/>
+    <sheet name="TestRolelistAndroid" r:id="rId19" sheetId="25"/>
+    <sheet name="TestIndustryListAndroid" r:id="rId20" sheetId="26"/>
+    <sheet name="TestTechnologylistAndroid" r:id="rId21" sheetId="27"/>
+    <sheet name="TestProductlistAndroid" r:id="rId22" sheetId="28"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="76">
   <si>
     <t>ID</t>
   </si>
@@ -191,13 +198,76 @@
     <t>Architects - Technical tag was found</t>
   </si>
   <si>
-    <t>Social &amp; Enterprise Mobility tag wasn't found</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence / Robotics tag wasn't found</t>
-  </si>
-  <si>
     <t>Social &amp; Enterprise Mobility tag was found</t>
+  </si>
+  <si>
+    <t>NewAnswerQ1Android</t>
+  </si>
+  <si>
+    <t>NewAnswerQ2Android</t>
+  </si>
+  <si>
+    <t>NewAnswerQ3Android</t>
+  </si>
+  <si>
+    <t>Add a complete new Answer for Q1</t>
+  </si>
+  <si>
+    <t>Add a complete new Answer for Q2</t>
+  </si>
+  <si>
+    <t>Add a complete new Answer for Q3</t>
+  </si>
+  <si>
+    <t>Question 1 answer was found</t>
+  </si>
+  <si>
+    <t>Question 2 answer was found</t>
+  </si>
+  <si>
+    <t>Question 3 answer was found</t>
+  </si>
+  <si>
+    <t>TestRolelistAndroid</t>
+  </si>
+  <si>
+    <t>TestIndustryListAndroid</t>
+  </si>
+  <si>
+    <t>TestTechnologylistAndroid</t>
+  </si>
+  <si>
+    <t>TestProductlistAndroid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Role tags List </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Industry tags List </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Technology tags List </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Product tags List </t>
+  </si>
+  <si>
+    <t>.NET wasn't found</t>
+  </si>
+  <si>
+    <t>2D wasn't found</t>
+  </si>
+  <si>
+    <t>Agile wasn't found</t>
+  </si>
+  <si>
+    <t>Aviation wasn't found</t>
+  </si>
+  <si>
+    <t>Aerospace &amp; Defence wasn't found</t>
+  </si>
+  <si>
+    <t>Internet of things wasn't found</t>
   </si>
 </sst>
 </file>
@@ -278,9 +348,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
@@ -315,7 +399,7 @@
     <xf applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="40">
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="3"/>
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="4"/>
@@ -340,6 +424,20 @@
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="23"/>
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="24"/>
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="25"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="26"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="27"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="28"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="29"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="30"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="31"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="32"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="33"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="34"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="35"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="36"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="37"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="38"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="39"/>
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
@@ -670,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -888,6 +986,104 @@
       </c>
       <c r="D15" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1143,8 +1339,8 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.76953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.23828125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1219,8 +1415,8 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.76953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="37.57421875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="37.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1266,7 +1462,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1287,7 +1483,316 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.1640625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+  </hyperlinks>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.76953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.07421875" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" width="31.33203125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+  </hyperlinks>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="27.1640625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+  </hyperlinks>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.83203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.33203125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+  </hyperlinks>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1342,7 +1847,7 @@
         <v>49</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1350,6 +1855,7 @@
     <hyperlink r:id="rId1" ref="B2"/>
   </hyperlinks>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1430,6 +1936,235 @@
   </hyperlinks>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.76953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="29.5234375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+  </hyperlinks>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.76953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.15234375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+  </hyperlinks>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.76953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.2421875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+  </hyperlinks>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>